<commit_message>
changed file structure and updated main file to clean up comments.
</commit_message>
<xml_diff>
--- a/Change Log Updated.xlsx
+++ b/Change Log Updated.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28800" windowHeight="12660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12660" windowWidth="28800"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="October" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="October" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="144525" fullCalcOnLoad="1"/>
@@ -16,8 +16,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ " numFmtId="164"/>
+    <numFmt formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ " numFmtId="165"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -491,212 +491,212 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="44">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="9" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="4" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="18" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="7" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="27" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="6"/>
+    <cellStyle builtinId="23" name="Check Cell" xfId="7"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="8"/>
+    <cellStyle builtinId="10" name="Note" xfId="9"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="10"/>
+    <cellStyle builtinId="44" name="60% - Accent4" xfId="11"/>
+    <cellStyle builtinId="9" name="Followed Hyperlink" xfId="12"/>
+    <cellStyle builtinId="39" name="40% - Accent3" xfId="13"/>
+    <cellStyle builtinId="11" name="Warning Text" xfId="14"/>
+    <cellStyle builtinId="35" name="40% - Accent2" xfId="15"/>
+    <cellStyle builtinId="15" name="Title" xfId="16"/>
+    <cellStyle builtinId="53" name="CExplanatory Text" xfId="17"/>
+    <cellStyle builtinId="16" name="Heading 1" xfId="18"/>
+    <cellStyle builtinId="18" name="Heading 3" xfId="19"/>
+    <cellStyle builtinId="19" name="Heading 4" xfId="20"/>
+    <cellStyle builtinId="20" name="Input" xfId="21"/>
+    <cellStyle builtinId="40" name="60% - Accent3" xfId="22"/>
+    <cellStyle builtinId="26" name="Good" xfId="23"/>
+    <cellStyle builtinId="21" name="Output" xfId="24"/>
+    <cellStyle builtinId="30" name="20% - Accent1" xfId="25"/>
+    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
+    <cellStyle builtinId="24" name="Linked Cell" xfId="27"/>
+    <cellStyle builtinId="25" name="Total" xfId="28"/>
+    <cellStyle builtinId="27" name="Bad" xfId="29"/>
+    <cellStyle builtinId="28" name="Neutral" xfId="30"/>
+    <cellStyle builtinId="29" name="Accent1" xfId="31"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="32"/>
+    <cellStyle builtinId="32" name="60% - Accent1" xfId="33"/>
+    <cellStyle builtinId="33" name="Accent2" xfId="34"/>
+    <cellStyle builtinId="34" name="20% - Accent2" xfId="35"/>
+    <cellStyle builtinId="50" name="20% - Accent6" xfId="36"/>
+    <cellStyle builtinId="36" name="60% - Accent2" xfId="37"/>
+    <cellStyle builtinId="37" name="Accent3" xfId="38"/>
+    <cellStyle builtinId="38" name="20% - Accent3" xfId="39"/>
+    <cellStyle builtinId="41" name="Accent4" xfId="40"/>
+    <cellStyle builtinId="42" name="20% - Accent4" xfId="41"/>
+    <cellStyle builtinId="43" name="40% - Accent4" xfId="42"/>
+    <cellStyle builtinId="45" name="Accent5" xfId="43"/>
+    <cellStyle builtinId="47" name="40% - Accent5" xfId="44"/>
+    <cellStyle builtinId="48" name="60% - Accent5" xfId="45"/>
+    <cellStyle builtinId="49" name="Accent6" xfId="46"/>
+    <cellStyle builtinId="51" name="40% - Accent6" xfId="47"/>
+    <cellStyle builtinId="52" name="60% - Accent6" xfId="48"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -896,7 +896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
@@ -907,14 +907,14 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.4285714285714" defaultRowHeight="15.75"/>
   <cols>
-    <col width="15.5714285714286" customWidth="1" min="1" max="1"/>
-    <col width="13.1428571428571" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="5.57142857142857" customWidth="1" min="4" max="4"/>
-    <col width="3.28571428571429" customWidth="1" min="5" max="5"/>
-    <col width="4.14285714285714" customWidth="1" min="6" max="6"/>
+    <col customWidth="1" max="1" min="1" width="15.5714285714286"/>
+    <col customWidth="1" max="2" min="2" width="13.1428571428571"/>
+    <col customWidth="1" max="3" min="3" width="15"/>
+    <col customWidth="1" max="4" min="4" width="5.57142857142857"/>
+    <col customWidth="1" max="5" min="5" width="3.28571428571429"/>
+    <col customWidth="1" max="6" min="6" width="4.14285714285714"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1176,13 +1176,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B6" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B7" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B8" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B9" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B10" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>